<commit_message>
Added examples to `testing_Rpackage.Rmd` for the summary uncertainty calculations + replicated some absolute and relative risk calculations in the newly created NIPH testing excel "example_road_noise_niph_test.xlsx"
</commit_message>
<xml_diff>
--- a/r_package/testing/input/noise_niph/example_road_noise_niph_test.xlsx
+++ b/r_package/testing/input/noise_niph/example_road_noise_niph_test.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19430" windowHeight="11630" tabRatio="895" activeTab="2"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19430" windowHeight="11630" tabRatio="895" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Absolute_risk_HA" sheetId="21" r:id="rId1"/>
     <sheet name="Absolute_risk_HSD" sheetId="18" r:id="rId2"/>
-    <sheet name="Relative_risk_IHD_WHO_2003a" sheetId="19" r:id="rId3"/>
-    <sheet name="Relative_risk_IHD_WHO_2003b" sheetId="20" r:id="rId4"/>
+    <sheet name="geo_id_1_rr_IHD_WHO_2003a" sheetId="22" r:id="rId3"/>
+    <sheet name="geo_id_2_rr_IHD_WHO_2003a" sheetId="19" r:id="rId4"/>
+    <sheet name="Relative_risk_IHD_WHO_2003b" sheetId="20" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="33">
   <si>
     <t>&lt; 55</t>
   </si>
@@ -147,7 +148,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="32" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -287,8 +288,81 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF808080"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF808080"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFBFBFBF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF808080"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -305,6 +379,18 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBFBFBF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6E0B4"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -377,7 +463,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -515,13 +601,70 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="16" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="22" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="23" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="27" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="22" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1393,10 +1536,422 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N13"/>
+  <sheetViews>
+    <sheetView topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="14" width="16.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="62" x14ac:dyDescent="0.35">
+      <c r="A1" s="90" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="91" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="90" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="90" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="90" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="92" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="92" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="90" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="92" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="92" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="92" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="93" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" s="93" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" s="93" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="94" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="95">
+        <v>53</v>
+      </c>
+      <c r="C2" s="96"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="98">
+        <f>E9-E8</f>
+        <v>4268785</v>
+      </c>
+      <c r="F2" s="99">
+        <f>E2/E9</f>
+        <v>0.81871831238486492</v>
+      </c>
+      <c r="G2" s="100">
+        <f>EXP((LN(1.08)/10)*(B2-53))</f>
+        <v>1</v>
+      </c>
+      <c r="H2" s="101">
+        <f>F2*G2</f>
+        <v>0.81871831238486492</v>
+      </c>
+      <c r="I2" s="102"/>
+      <c r="J2" s="102"/>
+      <c r="K2" s="102"/>
+      <c r="L2" s="103">
+        <v>5269.46</v>
+      </c>
+      <c r="M2" s="103">
+        <v>80092.63</v>
+      </c>
+      <c r="N2" s="103">
+        <v>85362.08</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="102" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="104">
+        <v>57.5</v>
+      </c>
+      <c r="C3" s="105">
+        <v>327900</v>
+      </c>
+      <c r="D3" s="105">
+        <v>59600</v>
+      </c>
+      <c r="E3" s="103">
+        <f>C3+D3</f>
+        <v>387500</v>
+      </c>
+      <c r="F3" s="99">
+        <f>E3/E9</f>
+        <v>7.4319354581956029E-2</v>
+      </c>
+      <c r="G3" s="100">
+        <f>EXP((LN(1.08)/10)*(B3-53))</f>
+        <v>1.0352391558831511</v>
+      </c>
+      <c r="H3" s="101">
+        <f>F3*G3</f>
+        <v>7.6938305903204759E-2</v>
+      </c>
+      <c r="I3" s="102"/>
+      <c r="J3" s="102"/>
+      <c r="K3" s="102"/>
+      <c r="L3" s="62"/>
+      <c r="M3" s="62"/>
+      <c r="N3" s="62"/>
+    </row>
+    <row r="4" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="102" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="104">
+        <v>62.5</v>
+      </c>
+      <c r="C4" s="105">
+        <v>236500</v>
+      </c>
+      <c r="D4" s="105">
+        <v>49500</v>
+      </c>
+      <c r="E4" s="103">
+        <f t="shared" ref="E4:E7" si="0">C4+D4</f>
+        <v>286000</v>
+      </c>
+      <c r="F4" s="99">
+        <f>E4/E9</f>
+        <v>5.4852478478553353E-2</v>
+      </c>
+      <c r="G4" s="100">
+        <f t="shared" ref="G4:G7" si="1">EXP((LN(1.08)/10)*(B4-53))</f>
+        <v>1.0758520895846009</v>
+      </c>
+      <c r="H4" s="101">
+        <f t="shared" ref="H4:H7" si="2">F4*G4</f>
+        <v>5.9013153590045976E-2</v>
+      </c>
+      <c r="I4" s="102"/>
+      <c r="J4" s="102"/>
+      <c r="K4" s="62"/>
+      <c r="L4" s="106"/>
+      <c r="M4" s="106"/>
+      <c r="N4" s="106"/>
+    </row>
+    <row r="5" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="102" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="104">
+        <v>67.5</v>
+      </c>
+      <c r="C5" s="105">
+        <v>167300</v>
+      </c>
+      <c r="D5" s="105">
+        <v>24500</v>
+      </c>
+      <c r="E5" s="103">
+        <f t="shared" si="0"/>
+        <v>191800</v>
+      </c>
+      <c r="F5" s="99">
+        <f>E5/E9</f>
+        <v>3.6785683119533334E-2</v>
+      </c>
+      <c r="G5" s="100">
+        <f t="shared" si="1"/>
+        <v>1.1180582883538033</v>
+      </c>
+      <c r="H5" s="101">
+        <f t="shared" si="2"/>
+        <v>4.1128537904550837E-2</v>
+      </c>
+      <c r="I5" s="102"/>
+      <c r="J5" s="102"/>
+      <c r="K5" s="62"/>
+      <c r="L5" s="106"/>
+      <c r="M5" s="106"/>
+      <c r="N5" s="106"/>
+    </row>
+    <row r="6" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="102" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="104">
+        <v>72.5</v>
+      </c>
+      <c r="C6" s="105">
+        <v>69400</v>
+      </c>
+      <c r="D6" s="105">
+        <v>2800</v>
+      </c>
+      <c r="E6" s="103">
+        <f t="shared" si="0"/>
+        <v>72200</v>
+      </c>
+      <c r="F6" s="99">
+        <f>E6/E9</f>
+        <v>1.384737393759284E-2</v>
+      </c>
+      <c r="G6" s="100">
+        <f t="shared" si="1"/>
+        <v>1.1619202567513689</v>
+      </c>
+      <c r="H6" s="101">
+        <f t="shared" si="2"/>
+        <v>1.6089544280900085E-2</v>
+      </c>
+      <c r="I6" s="102"/>
+      <c r="J6" s="107"/>
+      <c r="K6" s="102"/>
+      <c r="L6" s="62"/>
+      <c r="M6" s="62"/>
+      <c r="N6" s="62"/>
+    </row>
+    <row r="7" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="102" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="104">
+        <v>77.5</v>
+      </c>
+      <c r="C7" s="105">
+        <v>7700</v>
+      </c>
+      <c r="D7" s="105">
+        <v>0</v>
+      </c>
+      <c r="E7" s="103">
+        <f t="shared" si="0"/>
+        <v>7700</v>
+      </c>
+      <c r="F7" s="99">
+        <f>E7/E9</f>
+        <v>1.4767974974995133E-3</v>
+      </c>
+      <c r="G7" s="100">
+        <f t="shared" si="1"/>
+        <v>1.2075029514221076</v>
+      </c>
+      <c r="H7" s="101">
+        <f t="shared" si="2"/>
+        <v>1.783237336883445E-3</v>
+      </c>
+      <c r="I7" s="102"/>
+      <c r="J7" s="102"/>
+      <c r="K7" s="102"/>
+      <c r="L7" s="62"/>
+      <c r="M7" s="62"/>
+      <c r="N7" s="62"/>
+    </row>
+    <row r="8" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="108" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="108"/>
+      <c r="C8" s="109">
+        <f>SUM(C3:C7)</f>
+        <v>808800</v>
+      </c>
+      <c r="D8" s="109">
+        <f>SUM(D3:D7)</f>
+        <v>136400</v>
+      </c>
+      <c r="E8" s="110">
+        <f>SUM(E3:E7)</f>
+        <v>945200</v>
+      </c>
+      <c r="F8" s="111">
+        <f>E8/E9</f>
+        <v>0.18128168761513505</v>
+      </c>
+      <c r="G8" s="108"/>
+      <c r="H8" s="111">
+        <f>SUM((F2*G2+F3*G3+F4*G4+F5*G5+F6*G6+F7*G7)-1)/(F2*G2+F3*G3+F4*G4+F5*G5+F6*G6+F7*G7)*100</f>
+        <v>1.3486713310095881</v>
+      </c>
+      <c r="I8" s="112">
+        <f>L2*H8/100</f>
+        <v>71.067696319017841</v>
+      </c>
+      <c r="J8" s="112">
+        <f>M2*H8/100</f>
+        <v>1080.1863390615847</v>
+      </c>
+      <c r="K8" s="112">
+        <f>I8+J8</f>
+        <v>1151.2540353806025</v>
+      </c>
+      <c r="L8" s="62"/>
+      <c r="M8" s="62"/>
+      <c r="N8" s="62"/>
+    </row>
+    <row r="9" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="113" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="113"/>
+      <c r="C9" s="114"/>
+      <c r="D9" s="114"/>
+      <c r="E9" s="115">
+        <v>5213985</v>
+      </c>
+      <c r="F9" s="116">
+        <f>SUM(F2:F7)</f>
+        <v>1</v>
+      </c>
+      <c r="G9" s="113"/>
+      <c r="H9" s="113"/>
+      <c r="I9" s="113"/>
+      <c r="J9" s="113"/>
+      <c r="K9" s="113"/>
+      <c r="L9" s="62"/>
+      <c r="M9" s="62"/>
+      <c r="N9" s="62"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A10" s="117"/>
+      <c r="B10" s="117"/>
+      <c r="C10" s="118"/>
+      <c r="D10" s="118"/>
+      <c r="E10" s="118"/>
+      <c r="F10" s="119"/>
+      <c r="G10" s="62"/>
+      <c r="H10" s="62"/>
+      <c r="I10" s="62"/>
+      <c r="J10" s="62"/>
+      <c r="K10" s="62"/>
+      <c r="L10" s="62"/>
+      <c r="M10" s="62"/>
+      <c r="N10" s="62"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A11" s="117"/>
+      <c r="B11" s="117"/>
+      <c r="C11" s="118"/>
+      <c r="D11" s="118"/>
+      <c r="E11" s="118"/>
+      <c r="F11" s="120"/>
+      <c r="G11" s="121"/>
+      <c r="H11" s="121"/>
+      <c r="I11" s="62"/>
+      <c r="J11" s="62"/>
+      <c r="K11" s="62"/>
+      <c r="L11" s="62"/>
+      <c r="M11" s="62"/>
+      <c r="N11" s="62"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A12" s="117"/>
+      <c r="B12" s="117"/>
+      <c r="C12" s="118"/>
+      <c r="D12" s="118"/>
+      <c r="E12" s="118"/>
+      <c r="F12" s="122"/>
+      <c r="G12" s="122"/>
+      <c r="H12" s="123"/>
+      <c r="I12" s="62"/>
+      <c r="J12" s="62"/>
+      <c r="K12" s="62"/>
+      <c r="L12" s="62"/>
+      <c r="M12" s="62"/>
+      <c r="N12" s="62"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A13" s="124"/>
+      <c r="B13" s="124"/>
+      <c r="C13" s="124"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="62"/>
+      <c r="F13" s="122"/>
+      <c r="G13" s="122"/>
+      <c r="H13" s="123"/>
+      <c r="I13" s="62"/>
+      <c r="J13" s="62"/>
+      <c r="K13" s="62"/>
+      <c r="L13" s="62"/>
+      <c r="M13" s="62"/>
+      <c r="N13" s="62"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A13:C13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1744,7 +2299,7 @@
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="89" t="s">
+      <c r="A11" s="87" t="s">
         <v>31</v>
       </c>
       <c r="B11" s="11"/>
@@ -1768,17 +2323,17 @@
       <c r="H12" s="78"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A13" s="87"/>
-      <c r="B13" s="87"/>
-      <c r="C13" s="87"/>
+      <c r="A13" s="88"/>
+      <c r="B13" s="88"/>
+      <c r="C13" s="88"/>
       <c r="F13" s="77"/>
       <c r="G13" s="77"/>
       <c r="H13" s="78"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A14" s="88"/>
-      <c r="B14" s="88"/>
-      <c r="C14" s="88"/>
+      <c r="A14" s="89"/>
+      <c r="B14" s="89"/>
+      <c r="C14" s="89"/>
       <c r="F14" s="79"/>
       <c r="G14" s="79"/>
       <c r="H14" s="78"/>
@@ -1852,7 +2407,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R37"/>
   <sheetViews>
@@ -2300,9 +2855,9 @@
       <c r="K12" s="82"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A13" s="87"/>
-      <c r="B13" s="87"/>
-      <c r="C13" s="87"/>
+      <c r="A13" s="88"/>
+      <c r="B13" s="88"/>
+      <c r="C13" s="88"/>
       <c r="F13" s="77"/>
       <c r="G13" s="77"/>
       <c r="H13" s="77"/>
@@ -2311,9 +2866,9 @@
       <c r="K13" s="78"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A14" s="88"/>
-      <c r="B14" s="88"/>
-      <c r="C14" s="88"/>
+      <c r="A14" s="89"/>
+      <c r="B14" s="89"/>
+      <c r="C14" s="89"/>
       <c r="F14" s="79"/>
       <c r="G14" s="79"/>
       <c r="H14" s="79"/>
@@ -2451,6 +3006,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010000B17EB79AE2164A80F4AFE3B0051146" ma:contentTypeVersion="16" ma:contentTypeDescription="Opprett et nytt dokument." ma:contentTypeScope="" ma:versionID="6bdb926755f4c89fc32634e0fb424225">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9e7c1b5f-6b93-4ee4-9fa2-fda8f1b47cf5" xmlns:ns3="e0a242cb-cec1-4671-aa99-615488d5530e" xmlns:ns4="9d23e429-547e-4a13-8b71-070d02c5a1ec" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b0d894d6c78ef32a5fd57768bfb40a5e" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="9e7c1b5f-6b93-4ee4-9fa2-fda8f1b47cf5"/>
@@ -2688,15 +3252,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2737,6 +3292,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44A4E13C-9AD0-4A6A-9D51-20AD50148DE0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4AF6BACD-FB0D-4A79-B41F-209A25C08460}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2756,14 +3319,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44A4E13C-9AD0-4A6A-9D51-20AD50148DE0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA136E82-55D6-4201-8C86-EA83CE955D86}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Corrected example in `testing_Rpackage` + structured `get_risk_and_pop_fraction`
</commit_message>
<xml_diff>
--- a/r_package/testing/input/noise_niph/example_road_noise_niph_test.xlsx
+++ b/r_package/testing/input/noise_niph/example_road_noise_niph_test.xlsx
@@ -9,14 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19430" windowHeight="11630" tabRatio="895" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19430" windowHeight="11630" tabRatio="895" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Absolute_risk_HA" sheetId="21" r:id="rId1"/>
     <sheet name="Absolute_risk_HSD" sheetId="18" r:id="rId2"/>
     <sheet name="geo_id_1_rr_IHD_WHO_2003a" sheetId="22" r:id="rId3"/>
     <sheet name="geo_id_2_rr_IHD_WHO_2003a" sheetId="19" r:id="rId4"/>
-    <sheet name="Relative_risk_IHD_WHO_2003b" sheetId="20" r:id="rId5"/>
+    <sheet name="geo_id_3_rr_IHD_WHO_2003a (2)" sheetId="23" r:id="rId5"/>
+    <sheet name="Relative_risk_IHD_WHO_2003b" sheetId="20" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="33">
   <si>
     <t>&lt; 55</t>
   </si>
@@ -463,7 +464,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="125">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -602,9 +603,6 @@
     </xf>
     <xf numFmtId="164" fontId="16" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -663,6 +661,12 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1538,8 +1542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1547,303 +1551,303 @@
     <col min="1" max="14" width="16.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="62" x14ac:dyDescent="0.35">
-      <c r="A1" s="90" t="s">
+    <row r="1" spans="1:14" ht="31" x14ac:dyDescent="0.35">
+      <c r="A1" s="89" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="91" t="s">
+      <c r="B1" s="90" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="90" t="s">
+      <c r="C1" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="90" t="s">
+      <c r="D1" s="89" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="90" t="s">
+      <c r="E1" s="89" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="92" t="s">
+      <c r="F1" s="91" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="92" t="s">
+      <c r="G1" s="91" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="90" t="s">
+      <c r="H1" s="89" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="92" t="s">
+      <c r="I1" s="91" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="92" t="s">
+      <c r="J1" s="91" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="92" t="s">
+      <c r="K1" s="91" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="93" t="s">
+      <c r="L1" s="92" t="s">
         <v>26</v>
       </c>
-      <c r="M1" s="93" t="s">
+      <c r="M1" s="92" t="s">
         <v>27</v>
       </c>
-      <c r="N1" s="93" t="s">
+      <c r="N1" s="92" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="94" t="s">
+      <c r="A2" s="93" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="95">
+      <c r="B2" s="94">
         <v>53</v>
       </c>
-      <c r="C2" s="96"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="98">
+      <c r="C2" s="95"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="97">
         <f>E9-E8</f>
         <v>4268785</v>
       </c>
-      <c r="F2" s="99">
+      <c r="F2" s="98">
         <f>E2/E9</f>
         <v>0.81871831238486492</v>
       </c>
-      <c r="G2" s="100">
+      <c r="G2" s="99">
         <f>EXP((LN(1.08)/10)*(B2-53))</f>
         <v>1</v>
       </c>
-      <c r="H2" s="101">
+      <c r="H2" s="100">
         <f>F2*G2</f>
         <v>0.81871831238486492</v>
       </c>
-      <c r="I2" s="102"/>
-      <c r="J2" s="102"/>
-      <c r="K2" s="102"/>
-      <c r="L2" s="103">
+      <c r="I2" s="101"/>
+      <c r="J2" s="101"/>
+      <c r="K2" s="101"/>
+      <c r="L2" s="102">
         <v>5269.46</v>
       </c>
-      <c r="M2" s="103">
+      <c r="M2" s="102">
         <v>80092.63</v>
       </c>
-      <c r="N2" s="103">
+      <c r="N2" s="102">
         <v>85362.08</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="102" t="s">
+      <c r="A3" s="101" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="104">
+      <c r="B3" s="103">
         <v>57.5</v>
       </c>
-      <c r="C3" s="105">
+      <c r="C3" s="104">
         <v>327900</v>
       </c>
-      <c r="D3" s="105">
+      <c r="D3" s="104">
         <v>59600</v>
       </c>
-      <c r="E3" s="103">
+      <c r="E3" s="102">
         <f>C3+D3</f>
         <v>387500</v>
       </c>
-      <c r="F3" s="99">
+      <c r="F3" s="98">
         <f>E3/E9</f>
         <v>7.4319354581956029E-2</v>
       </c>
-      <c r="G3" s="100">
+      <c r="G3" s="99">
         <f>EXP((LN(1.08)/10)*(B3-53))</f>
         <v>1.0352391558831511</v>
       </c>
-      <c r="H3" s="101">
+      <c r="H3" s="100">
         <f>F3*G3</f>
         <v>7.6938305903204759E-2</v>
       </c>
-      <c r="I3" s="102"/>
-      <c r="J3" s="102"/>
-      <c r="K3" s="102"/>
+      <c r="I3" s="101"/>
+      <c r="J3" s="101"/>
+      <c r="K3" s="101"/>
       <c r="L3" s="62"/>
       <c r="M3" s="62"/>
       <c r="N3" s="62"/>
     </row>
     <row r="4" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="102" t="s">
+      <c r="A4" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="104">
+      <c r="B4" s="103">
         <v>62.5</v>
       </c>
-      <c r="C4" s="105">
+      <c r="C4" s="104">
         <v>236500</v>
       </c>
-      <c r="D4" s="105">
+      <c r="D4" s="104">
         <v>49500</v>
       </c>
-      <c r="E4" s="103">
+      <c r="E4" s="102">
         <f t="shared" ref="E4:E7" si="0">C4+D4</f>
         <v>286000</v>
       </c>
-      <c r="F4" s="99">
+      <c r="F4" s="98">
         <f>E4/E9</f>
         <v>5.4852478478553353E-2</v>
       </c>
-      <c r="G4" s="100">
+      <c r="G4" s="99">
         <f t="shared" ref="G4:G7" si="1">EXP((LN(1.08)/10)*(B4-53))</f>
         <v>1.0758520895846009</v>
       </c>
-      <c r="H4" s="101">
+      <c r="H4" s="100">
         <f t="shared" ref="H4:H7" si="2">F4*G4</f>
         <v>5.9013153590045976E-2</v>
       </c>
-      <c r="I4" s="102"/>
-      <c r="J4" s="102"/>
+      <c r="I4" s="101"/>
+      <c r="J4" s="101"/>
       <c r="K4" s="62"/>
-      <c r="L4" s="106"/>
-      <c r="M4" s="106"/>
-      <c r="N4" s="106"/>
+      <c r="L4" s="105"/>
+      <c r="M4" s="105"/>
+      <c r="N4" s="105"/>
     </row>
     <row r="5" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="102" t="s">
+      <c r="A5" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="104">
+      <c r="B5" s="103">
         <v>67.5</v>
       </c>
-      <c r="C5" s="105">
+      <c r="C5" s="104">
         <v>167300</v>
       </c>
-      <c r="D5" s="105">
+      <c r="D5" s="104">
         <v>24500</v>
       </c>
-      <c r="E5" s="103">
+      <c r="E5" s="102">
         <f t="shared" si="0"/>
         <v>191800</v>
       </c>
-      <c r="F5" s="99">
+      <c r="F5" s="98">
         <f>E5/E9</f>
         <v>3.6785683119533334E-2</v>
       </c>
-      <c r="G5" s="100">
+      <c r="G5" s="99">
         <f t="shared" si="1"/>
         <v>1.1180582883538033</v>
       </c>
-      <c r="H5" s="101">
+      <c r="H5" s="100">
         <f t="shared" si="2"/>
         <v>4.1128537904550837E-2</v>
       </c>
-      <c r="I5" s="102"/>
-      <c r="J5" s="102"/>
+      <c r="I5" s="101"/>
+      <c r="J5" s="101"/>
       <c r="K5" s="62"/>
-      <c r="L5" s="106"/>
-      <c r="M5" s="106"/>
-      <c r="N5" s="106"/>
+      <c r="L5" s="105"/>
+      <c r="M5" s="105"/>
+      <c r="N5" s="105"/>
     </row>
     <row r="6" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="102" t="s">
+      <c r="A6" s="101" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="104">
+      <c r="B6" s="103">
         <v>72.5</v>
       </c>
-      <c r="C6" s="105">
+      <c r="C6" s="104">
         <v>69400</v>
       </c>
-      <c r="D6" s="105">
+      <c r="D6" s="104">
         <v>2800</v>
       </c>
-      <c r="E6" s="103">
+      <c r="E6" s="102">
         <f t="shared" si="0"/>
         <v>72200</v>
       </c>
-      <c r="F6" s="99">
+      <c r="F6" s="98">
         <f>E6/E9</f>
         <v>1.384737393759284E-2</v>
       </c>
-      <c r="G6" s="100">
+      <c r="G6" s="99">
         <f t="shared" si="1"/>
         <v>1.1619202567513689</v>
       </c>
-      <c r="H6" s="101">
+      <c r="H6" s="100">
         <f t="shared" si="2"/>
         <v>1.6089544280900085E-2</v>
       </c>
-      <c r="I6" s="102"/>
-      <c r="J6" s="107"/>
-      <c r="K6" s="102"/>
+      <c r="I6" s="101"/>
+      <c r="J6" s="106"/>
+      <c r="K6" s="101"/>
       <c r="L6" s="62"/>
       <c r="M6" s="62"/>
       <c r="N6" s="62"/>
     </row>
     <row r="7" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="102" t="s">
+      <c r="A7" s="101" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="104">
+      <c r="B7" s="103">
         <v>77.5</v>
       </c>
-      <c r="C7" s="105">
+      <c r="C7" s="104">
         <v>7700</v>
       </c>
-      <c r="D7" s="105">
+      <c r="D7" s="104">
         <v>0</v>
       </c>
-      <c r="E7" s="103">
+      <c r="E7" s="102">
         <f t="shared" si="0"/>
         <v>7700</v>
       </c>
-      <c r="F7" s="99">
+      <c r="F7" s="98">
         <f>E7/E9</f>
         <v>1.4767974974995133E-3</v>
       </c>
-      <c r="G7" s="100">
+      <c r="G7" s="99">
         <f t="shared" si="1"/>
         <v>1.2075029514221076</v>
       </c>
-      <c r="H7" s="101">
+      <c r="H7" s="100">
         <f t="shared" si="2"/>
         <v>1.783237336883445E-3</v>
       </c>
-      <c r="I7" s="102"/>
-      <c r="J7" s="102"/>
-      <c r="K7" s="102"/>
+      <c r="I7" s="101"/>
+      <c r="J7" s="101"/>
+      <c r="K7" s="101"/>
       <c r="L7" s="62"/>
       <c r="M7" s="62"/>
       <c r="N7" s="62"/>
     </row>
     <row r="8" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="108" t="s">
+      <c r="A8" s="107" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="108"/>
-      <c r="C8" s="109">
+      <c r="B8" s="107"/>
+      <c r="C8" s="108">
         <f>SUM(C3:C7)</f>
         <v>808800</v>
       </c>
-      <c r="D8" s="109">
+      <c r="D8" s="108">
         <f>SUM(D3:D7)</f>
         <v>136400</v>
       </c>
-      <c r="E8" s="110">
+      <c r="E8" s="109">
         <f>SUM(E3:E7)</f>
         <v>945200</v>
       </c>
-      <c r="F8" s="111">
+      <c r="F8" s="110">
         <f>E8/E9</f>
         <v>0.18128168761513505</v>
       </c>
-      <c r="G8" s="108"/>
-      <c r="H8" s="111">
+      <c r="G8" s="107"/>
+      <c r="H8" s="110">
         <f>SUM((F2*G2+F3*G3+F4*G4+F5*G5+F6*G6+F7*G7)-1)/(F2*G2+F3*G3+F4*G4+F5*G5+F6*G6+F7*G7)*100</f>
         <v>1.3486713310095881</v>
       </c>
-      <c r="I8" s="112">
+      <c r="I8" s="111">
         <f>L2*H8/100</f>
         <v>71.067696319017841</v>
       </c>
-      <c r="J8" s="112">
+      <c r="J8" s="111">
         <f>M2*H8/100</f>
         <v>1080.1863390615847</v>
       </c>
-      <c r="K8" s="112">
+      <c r="K8" s="111">
         <f>I8+J8</f>
         <v>1151.2540353806025</v>
       </c>
@@ -1852,35 +1856,35 @@
       <c r="N8" s="62"/>
     </row>
     <row r="9" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="113" t="s">
+      <c r="A9" s="112" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="113"/>
-      <c r="C9" s="114"/>
-      <c r="D9" s="114"/>
-      <c r="E9" s="115">
+      <c r="B9" s="112"/>
+      <c r="C9" s="113"/>
+      <c r="D9" s="113"/>
+      <c r="E9" s="114">
         <v>5213985</v>
       </c>
-      <c r="F9" s="116">
+      <c r="F9" s="115">
         <f>SUM(F2:F7)</f>
         <v>1</v>
       </c>
-      <c r="G9" s="113"/>
-      <c r="H9" s="113"/>
-      <c r="I9" s="113"/>
-      <c r="J9" s="113"/>
-      <c r="K9" s="113"/>
+      <c r="G9" s="112"/>
+      <c r="H9" s="112"/>
+      <c r="I9" s="112"/>
+      <c r="J9" s="112"/>
+      <c r="K9" s="112"/>
       <c r="L9" s="62"/>
       <c r="M9" s="62"/>
       <c r="N9" s="62"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A10" s="117"/>
-      <c r="B10" s="117"/>
-      <c r="C10" s="118"/>
-      <c r="D10" s="118"/>
-      <c r="E10" s="118"/>
-      <c r="F10" s="119"/>
+      <c r="A10" s="116"/>
+      <c r="B10" s="116"/>
+      <c r="C10" s="117"/>
+      <c r="D10" s="117"/>
+      <c r="E10" s="117"/>
+      <c r="F10" s="118"/>
       <c r="G10" s="62"/>
       <c r="H10" s="62"/>
       <c r="I10" s="62"/>
@@ -1891,14 +1895,14 @@
       <c r="N10" s="62"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A11" s="117"/>
-      <c r="B11" s="117"/>
-      <c r="C11" s="118"/>
-      <c r="D11" s="118"/>
-      <c r="E11" s="118"/>
-      <c r="F11" s="120"/>
-      <c r="G11" s="121"/>
-      <c r="H11" s="121"/>
+      <c r="A11" s="116"/>
+      <c r="B11" s="116"/>
+      <c r="C11" s="117"/>
+      <c r="D11" s="117"/>
+      <c r="E11" s="117"/>
+      <c r="F11" s="119"/>
+      <c r="G11" s="120"/>
+      <c r="H11" s="120"/>
       <c r="I11" s="62"/>
       <c r="J11" s="62"/>
       <c r="K11" s="62"/>
@@ -1907,14 +1911,14 @@
       <c r="N11" s="62"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A12" s="117"/>
-      <c r="B12" s="117"/>
-      <c r="C12" s="118"/>
-      <c r="D12" s="118"/>
-      <c r="E12" s="118"/>
-      <c r="F12" s="122"/>
-      <c r="G12" s="122"/>
-      <c r="H12" s="123"/>
+      <c r="A12" s="116"/>
+      <c r="B12" s="116"/>
+      <c r="C12" s="117"/>
+      <c r="D12" s="117"/>
+      <c r="E12" s="117"/>
+      <c r="F12" s="121"/>
+      <c r="G12" s="121"/>
+      <c r="H12" s="122"/>
       <c r="I12" s="62"/>
       <c r="J12" s="62"/>
       <c r="K12" s="62"/>
@@ -1923,14 +1927,14 @@
       <c r="N12" s="62"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A13" s="124"/>
-      <c r="B13" s="124"/>
-      <c r="C13" s="124"/>
+      <c r="A13" s="123"/>
+      <c r="B13" s="123"/>
+      <c r="C13" s="123"/>
       <c r="D13" s="62"/>
       <c r="E13" s="62"/>
-      <c r="F13" s="122"/>
-      <c r="G13" s="122"/>
-      <c r="H13" s="123"/>
+      <c r="F13" s="121"/>
+      <c r="G13" s="121"/>
+      <c r="H13" s="122"/>
       <c r="I13" s="62"/>
       <c r="J13" s="62"/>
       <c r="K13" s="62"/>
@@ -1950,8 +1954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2032,7 +2036,7 @@
       </c>
       <c r="F2" s="33">
         <f>(E2/E9) + A16</f>
-        <v>0.9187183123848649</v>
+        <v>0.81871831238486492</v>
       </c>
       <c r="G2" s="72">
         <f>EXP((LN(1.08)/10)*(B2-53))</f>
@@ -2040,7 +2044,7 @@
       </c>
       <c r="H2" s="34">
         <f>F2*G2</f>
-        <v>0.95476007693671294</v>
+        <v>0.85083702848258025</v>
       </c>
       <c r="I2" s="18"/>
       <c r="J2" s="18"/>
@@ -2075,7 +2079,7 @@
       </c>
       <c r="F3" s="33">
         <f xml:space="preserve"> (E3/E9) + A16</f>
-        <v>0.17431935458195602</v>
+        <v>7.4319354581956029E-2</v>
       </c>
       <c r="G3" s="72">
         <f>EXP((LN(1.08)/10)*(B3-53))</f>
@@ -2083,7 +2087,7 @@
       </c>
       <c r="H3" s="34">
         <f>F3*G3</f>
-        <v>0.18754184188203635</v>
+        <v>7.9956632923576271E-2</v>
       </c>
       <c r="I3" s="18"/>
       <c r="J3" s="18"/>
@@ -2109,7 +2113,7 @@
       </c>
       <c r="F4" s="33">
         <f xml:space="preserve"> (E4/E9) + A16</f>
-        <v>0.15485247847855335</v>
+        <v>5.4852478478553353E-2</v>
       </c>
       <c r="G4" s="72">
         <f t="shared" ref="G4:G7" si="1">EXP((LN(1.08)/10)*(B4-53))</f>
@@ -2117,7 +2121,7 @@
       </c>
       <c r="H4" s="34">
         <f t="shared" ref="H4:H7" si="2">F4*G4</f>
-        <v>0.17313409703507551</v>
+        <v>6.1328268199695196E-2</v>
       </c>
       <c r="I4" s="18"/>
       <c r="J4" s="18"/>
@@ -2146,7 +2150,7 @@
       </c>
       <c r="F5" s="33">
         <f xml:space="preserve"> (E5/E9) + A16</f>
-        <v>0.13678568311953335</v>
+        <v>3.6785683119533334E-2</v>
       </c>
       <c r="G5" s="72">
         <f t="shared" si="1"/>
@@ -2154,7 +2158,7 @@
       </c>
       <c r="H5" s="34">
         <f t="shared" si="2"/>
-        <v>0.15893405605015956</v>
+        <v>4.2742030375022666E-2</v>
       </c>
       <c r="I5" s="18"/>
       <c r="J5" s="18"/>
@@ -2183,7 +2187,7 @@
       </c>
       <c r="F6" s="33">
         <f xml:space="preserve"> (E6/E9) + A16</f>
-        <v>0.11384737393759284</v>
+        <v>1.384737393759284E-2</v>
       </c>
       <c r="G6" s="72">
         <f t="shared" si="1"/>
@@ -2191,7 +2195,7 @@
       </c>
       <c r="H6" s="34">
         <f t="shared" si="2"/>
-        <v>0.13747104004129967</v>
+        <v>1.6720744899088927E-2</v>
       </c>
       <c r="I6" s="18"/>
       <c r="J6" s="19"/>
@@ -2217,7 +2221,7 @@
       </c>
       <c r="F7" s="33">
         <f xml:space="preserve"> (E7/E9) + A16</f>
-        <v>0.10147679749749952</v>
+        <v>1.4767974974995133E-3</v>
       </c>
       <c r="G7" s="72">
         <f t="shared" si="1"/>
@@ -2225,7 +2229,7 @@
       </c>
       <c r="H7" s="34">
         <f t="shared" si="2"/>
-        <v>0.12734058233080942</v>
+        <v>1.8531946016615668E-3</v>
       </c>
       <c r="I7" s="18"/>
       <c r="J7" s="18"/>
@@ -2255,19 +2259,19 @@
       <c r="G8" s="36"/>
       <c r="H8" s="35">
         <f>SUM((F2*G2+F3*G3+F4*G4+F5*G5+F6*G6+F7*G7)-1)/(F2*G2+F3*G3+F4*G4+F5*G5+F6*G6+F7*G7)*100</f>
-        <v>42.501694717052892</v>
+        <v>5.0727147284069236</v>
       </c>
       <c r="I8" s="38">
         <f>L2*H8/100</f>
-        <v>2239.6098024372154</v>
+        <v>267.30467352751145</v>
       </c>
       <c r="J8" s="38">
         <f>M2*H8/100</f>
-        <v>34040.725093458721</v>
+        <v>4062.870638378462</v>
       </c>
       <c r="K8" s="38">
         <f>I8+J8</f>
-        <v>36280.33489589594</v>
+        <v>4330.1753119059731</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
@@ -2282,7 +2286,7 @@
       </c>
       <c r="F9" s="39">
         <f>SUM(F2:F7)</f>
-        <v>1.6</v>
+        <v>1</v>
       </c>
       <c r="G9" s="40"/>
       <c r="H9" s="40"/>
@@ -2323,17 +2327,17 @@
       <c r="H12" s="78"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A13" s="88"/>
-      <c r="B13" s="88"/>
-      <c r="C13" s="88"/>
+      <c r="A13" s="124"/>
+      <c r="B13" s="124"/>
+      <c r="C13" s="124"/>
       <c r="F13" s="77"/>
       <c r="G13" s="77"/>
       <c r="H13" s="78"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A14" s="89"/>
-      <c r="B14" s="89"/>
-      <c r="C14" s="89"/>
+      <c r="A14" s="125"/>
+      <c r="B14" s="125"/>
+      <c r="C14" s="125"/>
       <c r="F14" s="79"/>
       <c r="G14" s="79"/>
       <c r="H14" s="78"/>
@@ -2347,7 +2351,7 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" s="67">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="B16" s="68"/>
       <c r="C16" s="69"/>
@@ -2408,6 +2412,467 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="15.81640625" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" customWidth="1"/>
+    <col min="4" max="4" width="19.54296875" customWidth="1"/>
+    <col min="5" max="5" width="15.453125" customWidth="1"/>
+    <col min="6" max="6" width="15.7265625" customWidth="1"/>
+    <col min="7" max="7" width="21.26953125" customWidth="1"/>
+    <col min="8" max="8" width="16.81640625" customWidth="1"/>
+    <col min="11" max="11" width="13.1796875" customWidth="1"/>
+    <col min="12" max="12" width="23.54296875" customWidth="1"/>
+    <col min="13" max="13" width="21.54296875" customWidth="1"/>
+    <col min="14" max="14" width="21.453125" customWidth="1"/>
+    <col min="15" max="15" width="12.453125" customWidth="1"/>
+    <col min="17" max="17" width="10.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+      <c r="A1" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="73" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" s="73" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" s="73" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="58">
+        <f>53 + A12</f>
+        <v>63</v>
+      </c>
+      <c r="C2" s="46"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="29">
+        <f>E9-E8</f>
+        <v>4268785</v>
+      </c>
+      <c r="F2" s="33">
+        <f>(E2/E9) + A16</f>
+        <v>0.81871831238486492</v>
+      </c>
+      <c r="G2" s="72">
+        <f>EXP((LN(1.08)/10)*(B2-53))</f>
+        <v>1.08</v>
+      </c>
+      <c r="H2" s="34">
+        <f>F2*G2</f>
+        <v>0.88421577737565416</v>
+      </c>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="74">
+        <v>5269.46</v>
+      </c>
+      <c r="M2" s="74">
+        <v>80092.63</v>
+      </c>
+      <c r="N2" s="74">
+        <v>85362.08</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="59">
+        <f xml:space="preserve"> 57.5 + A12</f>
+        <v>67.5</v>
+      </c>
+      <c r="C3" s="48">
+        <v>327900</v>
+      </c>
+      <c r="D3" s="48">
+        <v>59600</v>
+      </c>
+      <c r="E3" s="30">
+        <f>C3+D3</f>
+        <v>387500</v>
+      </c>
+      <c r="F3" s="33">
+        <f xml:space="preserve"> (E3/E9) + A16</f>
+        <v>7.4319354581956029E-2</v>
+      </c>
+      <c r="G3" s="72">
+        <f>EXP((LN(1.08)/10)*(B3-53))</f>
+        <v>1.1180582883538033</v>
+      </c>
+      <c r="H3" s="34">
+        <f>F3*G3</f>
+        <v>8.3093370375461148E-2</v>
+      </c>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+    </row>
+    <row r="4" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="59">
+        <f xml:space="preserve"> 62.5 + A12</f>
+        <v>72.5</v>
+      </c>
+      <c r="C4" s="48">
+        <v>236500</v>
+      </c>
+      <c r="D4" s="48">
+        <v>49500</v>
+      </c>
+      <c r="E4" s="30">
+        <f t="shared" ref="E4:E7" si="0">C4+D4</f>
+        <v>286000</v>
+      </c>
+      <c r="F4" s="33">
+        <f xml:space="preserve"> (E4/E9) + A16</f>
+        <v>5.4852478478553353E-2</v>
+      </c>
+      <c r="G4" s="72">
+        <f t="shared" ref="G4:G7" si="1">EXP((LN(1.08)/10)*(B4-53))</f>
+        <v>1.1619202567513689</v>
+      </c>
+      <c r="H4" s="34">
+        <f t="shared" ref="H4:H7" si="2">F4*G4</f>
+        <v>6.373420587724965E-2</v>
+      </c>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="L4" s="41"/>
+      <c r="M4" s="41"/>
+      <c r="N4" s="41"/>
+      <c r="O4" s="42"/>
+    </row>
+    <row r="5" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="59">
+        <f xml:space="preserve"> 67.5+ A12</f>
+        <v>77.5</v>
+      </c>
+      <c r="C5" s="48">
+        <v>167300</v>
+      </c>
+      <c r="D5" s="48">
+        <v>24500</v>
+      </c>
+      <c r="E5" s="30">
+        <f t="shared" si="0"/>
+        <v>191800</v>
+      </c>
+      <c r="F5" s="33">
+        <f xml:space="preserve"> (E5/E9) + A16</f>
+        <v>3.6785683119533334E-2</v>
+      </c>
+      <c r="G5" s="72">
+        <f t="shared" si="1"/>
+        <v>1.2075029514221076</v>
+      </c>
+      <c r="H5" s="34">
+        <f t="shared" si="2"/>
+        <v>4.4418820936914905E-2</v>
+      </c>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="L5" s="41"/>
+      <c r="M5" s="41"/>
+      <c r="N5" s="41"/>
+      <c r="O5" s="42"/>
+    </row>
+    <row r="6" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="59">
+        <f xml:space="preserve"> 72.5+ A12</f>
+        <v>82.5</v>
+      </c>
+      <c r="C6" s="48">
+        <v>69400</v>
+      </c>
+      <c r="D6" s="48">
+        <v>2800</v>
+      </c>
+      <c r="E6" s="30">
+        <f t="shared" si="0"/>
+        <v>72200</v>
+      </c>
+      <c r="F6" s="33">
+        <f xml:space="preserve"> (E6/E9) + A16</f>
+        <v>1.384737393759284E-2</v>
+      </c>
+      <c r="G6" s="72">
+        <f t="shared" si="1"/>
+        <v>1.2548738772914785</v>
+      </c>
+      <c r="H6" s="34">
+        <f t="shared" si="2"/>
+        <v>1.7376707823372094E-2</v>
+      </c>
+      <c r="I6" s="18"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="18"/>
+    </row>
+    <row r="7" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="60">
+        <f xml:space="preserve"> 77.5 + A12</f>
+        <v>87.5</v>
+      </c>
+      <c r="C7" s="48">
+        <v>7700</v>
+      </c>
+      <c r="D7" s="48">
+        <v>0</v>
+      </c>
+      <c r="E7" s="30">
+        <f t="shared" si="0"/>
+        <v>7700</v>
+      </c>
+      <c r="F7" s="33">
+        <f xml:space="preserve"> (E7/E9) + A16</f>
+        <v>1.4767974974995133E-3</v>
+      </c>
+      <c r="G7" s="72">
+        <f t="shared" si="1"/>
+        <v>1.3041031875358762</v>
+      </c>
+      <c r="H7" s="34">
+        <f t="shared" si="2"/>
+        <v>1.9258963238341204E-3</v>
+      </c>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+    </row>
+    <row r="8" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="21"/>
+      <c r="C8" s="49">
+        <f>SUM(C3:C7)</f>
+        <v>808800</v>
+      </c>
+      <c r="D8" s="49">
+        <f>SUM(D3:D7)</f>
+        <v>136400</v>
+      </c>
+      <c r="E8" s="28">
+        <f>SUM(E3:E7)</f>
+        <v>945200</v>
+      </c>
+      <c r="F8" s="35">
+        <f>E8/E9</f>
+        <v>0.18128168761513505</v>
+      </c>
+      <c r="G8" s="36"/>
+      <c r="H8" s="35">
+        <f>SUM((F2*G2+F3*G3+F4*G4+F5*G5+F6*G6+F7*G7)-1)/(F2*G2+F3*G3+F4*G4+F5*G5+F6*G6+F7*G7)*100</f>
+        <v>8.6561771583422509</v>
+      </c>
+      <c r="I8" s="38">
+        <f>L2*H8/100</f>
+        <v>456.13379288798154</v>
+      </c>
+      <c r="J8" s="38">
+        <f>M2*H8/100</f>
+        <v>6932.9599435755736</v>
+      </c>
+      <c r="K8" s="38">
+        <f>I8+J8</f>
+        <v>7389.0937364635547</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="22"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="50">
+        <v>5213985</v>
+      </c>
+      <c r="F9" s="39">
+        <f>SUM(F2:F7)</f>
+        <v>1</v>
+      </c>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="40"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="87" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="11"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="75"/>
+      <c r="G11" s="76"/>
+      <c r="H11" s="76"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A12" s="62">
+        <v>10</v>
+      </c>
+      <c r="B12" s="62"/>
+      <c r="C12" s="63"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="77"/>
+      <c r="G12" s="77"/>
+      <c r="H12" s="78"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A13" s="124"/>
+      <c r="B13" s="124"/>
+      <c r="C13" s="124"/>
+      <c r="F13" s="77"/>
+      <c r="G13" s="77"/>
+      <c r="H13" s="78"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A14" s="125"/>
+      <c r="B14" s="125"/>
+      <c r="C14" s="125"/>
+      <c r="F14" s="79"/>
+      <c r="G14" s="79"/>
+      <c r="H14" s="78"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A15" s="88" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="65"/>
+      <c r="C15" s="66"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A16" s="67">
+        <v>0</v>
+      </c>
+      <c r="B16" s="68"/>
+      <c r="C16" s="69"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="67"/>
+      <c r="B17" s="56"/>
+      <c r="C17" s="69"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="67"/>
+      <c r="B18" s="68"/>
+      <c r="C18" s="69"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="67"/>
+      <c r="B19" s="68"/>
+      <c r="C19" s="69"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="66"/>
+      <c r="B20" s="70"/>
+      <c r="C20" s="70"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="67"/>
+      <c r="B21" s="67"/>
+      <c r="C21" s="67"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" s="67"/>
+      <c r="B22" s="67"/>
+      <c r="C22" s="67"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" s="71"/>
+      <c r="B23" s="67"/>
+      <c r="C23" s="67"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" s="67"/>
+      <c r="B24" s="67"/>
+      <c r="C24" s="67"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" s="67"/>
+      <c r="B25" s="67"/>
+      <c r="C25" s="67"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A14:C14"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R37"/>
   <sheetViews>
@@ -2855,9 +3320,9 @@
       <c r="K12" s="82"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A13" s="88"/>
-      <c r="B13" s="88"/>
-      <c r="C13" s="88"/>
+      <c r="A13" s="124"/>
+      <c r="B13" s="124"/>
+      <c r="C13" s="124"/>
       <c r="F13" s="77"/>
       <c r="G13" s="77"/>
       <c r="H13" s="77"/>
@@ -2866,9 +3331,9 @@
       <c r="K13" s="78"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A14" s="89"/>
-      <c r="B14" s="89"/>
-      <c r="C14" s="89"/>
+      <c r="A14" s="125"/>
+      <c r="B14" s="125"/>
+      <c r="C14" s="125"/>
       <c r="F14" s="79"/>
       <c r="G14" s="79"/>
       <c r="H14" s="79"/>
@@ -3006,12 +3471,42 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <FHI_TopicTaxHTField xmlns="9e7c1b5f-6b93-4ee4-9fa2-fda8f1b47cf5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Støy</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">8f2d7361-ae3f-42e5-b515-973ba07fa140</TermId>
+        </TermInfo>
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Sykdomsbyrde</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">1cb2573e-d91b-47cf-a8ed-abd0332371f0</TermId>
+        </TermInfo>
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Miljø og helse</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">87be7d37-248c-4b3c-9204-980558e4f787</TermId>
+        </TermInfo>
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Miljøeksponering</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">d9196c48-ce51-47cd-b0d2-6ebc45d8709a</TermId>
+        </TermInfo>
+      </Terms>
+    </FHI_TopicTaxHTField>
+    <TaxCatchAll xmlns="e0a242cb-cec1-4671-aa99-615488d5530e">
+      <Value>15</Value>
+      <Value>10</Value>
+      <Value>2</Value>
+      <Value>1</Value>
+    </TaxCatchAll>
+    <TaxKeywordTaxHTField xmlns="e0a242cb-cec1-4671-aa99-615488d5530e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9d23e429-547e-4a13-8b71-070d02c5a1ec">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3253,48 +3748,22 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <FHI_TopicTaxHTField xmlns="9e7c1b5f-6b93-4ee4-9fa2-fda8f1b47cf5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Støy</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">8f2d7361-ae3f-42e5-b515-973ba07fa140</TermId>
-        </TermInfo>
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Sykdomsbyrde</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">1cb2573e-d91b-47cf-a8ed-abd0332371f0</TermId>
-        </TermInfo>
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Miljø og helse</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">87be7d37-248c-4b3c-9204-980558e4f787</TermId>
-        </TermInfo>
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Miljøeksponering</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">d9196c48-ce51-47cd-b0d2-6ebc45d8709a</TermId>
-        </TermInfo>
-      </Terms>
-    </FHI_TopicTaxHTField>
-    <TaxCatchAll xmlns="e0a242cb-cec1-4671-aa99-615488d5530e">
-      <Value>15</Value>
-      <Value>10</Value>
-      <Value>2</Value>
-      <Value>1</Value>
-    </TaxCatchAll>
-    <TaxKeywordTaxHTField xmlns="e0a242cb-cec1-4671-aa99-615488d5530e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9d23e429-547e-4a13-8b71-070d02c5a1ec">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44A4E13C-9AD0-4A6A-9D51-20AD50148DE0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA136E82-55D6-4201-8C86-EA83CE955D86}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9e7c1b5f-6b93-4ee4-9fa2-fda8f1b47cf5"/>
+    <ds:schemaRef ds:uri="e0a242cb-cec1-4671-aa99-615488d5530e"/>
+    <ds:schemaRef ds:uri="9d23e429-547e-4a13-8b71-070d02c5a1ec"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3320,13 +3789,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA136E82-55D6-4201-8C86-EA83CE955D86}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44A4E13C-9AD0-4A6A-9D51-20AD50148DE0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9e7c1b5f-6b93-4ee4-9fa2-fda8f1b47cf5"/>
-    <ds:schemaRef ds:uri="e0a242cb-cec1-4671-aa99-615488d5530e"/>
-    <ds:schemaRef ds:uri="9d23e429-547e-4a13-8b71-070d02c5a1ec"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>